<commit_message>
Ajout de la transmission au fonctionnement global
</commit_message>
<xml_diff>
--- a/Dépendances.xlsx
+++ b/Dépendances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gdefr\Documents\2.Travail\INSA\4A\S7\BE Périphériques\BE_Periph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF377884-D813-481A-A14E-FBD960BFFE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795BBF9E-8376-462A-A91F-6BFA4B8C8C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dépendances HW" sheetId="1" r:id="rId1"/>
@@ -215,13 +215,13 @@
     <t>Actionneur</t>
   </si>
   <si>
-    <t>Sorties</t>
-  </si>
-  <si>
     <t>Pérpih.</t>
   </si>
   <si>
     <t>Pin</t>
+  </si>
+  <si>
+    <t>Entrées/Sorties</t>
   </si>
 </sst>
 </file>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -560,13 +560,13 @@
         <v>63</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -795,17 +795,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:E16">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
@@ -819,7 +819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E5AC77-F771-4A1D-B752-DF5B8CA98077}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>